<commit_message>
Add 'Strategy' Column to compared results excel
</commit_message>
<xml_diff>
--- a/Code/Data/DAX30/DAX30_returns_compared.xlsx
+++ b/Code/Data/DAX30/DAX30_returns_compared.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,20 +446,25 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Strategy</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Return</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Return_with_prediction</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>pct_change</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>mean_pct_change</t>
         </is>
@@ -479,16 +484,21 @@
           <t>2007-01-01</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Min volatility (Markowitz)</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>0.1267918748682099</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.1557847562796525</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>22.86651367966473</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>28.29691404819258</v>
       </c>
     </row>
@@ -506,16 +516,21 @@
           <t>2007-01-01</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Sharpe Ratio</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>0.1426424084643571</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>0.1648544851735231</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>15.57186039432043</v>
       </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -531,16 +546,21 @@
           <t>2008-01-01</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Min volatility (Markowitz)</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>-0.4063143513274387</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>-0.425026795304223</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>4.605410543745326</v>
       </c>
-      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -556,16 +576,21 @@
           <t>2008-01-01</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Sharpe Ratio</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
         <v>-0.4232244901888082</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>-0.4735135007878499</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>11.88234891052898</v>
       </c>
-      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -581,16 +606,21 @@
           <t>2009-01-01</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Min volatility (Markowitz)</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
         <v>0.2756922458683215</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>0.2493987862540644</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>-9.537250324702855</v>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -606,16 +636,21 @@
           <t>2009-01-01</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Sharpe Ratio</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
         <v>0.1852108248257389</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>0.5819789218863062</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>214.2251120764017</v>
       </c>
-      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -631,16 +666,21 @@
           <t>2010-01-01</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Min volatility (Markowitz)</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
         <v>0.1404406979708444</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>0.188813882466975</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>34.443850817498</v>
       </c>
-      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -656,16 +696,21 @@
           <t>2010-01-01</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Sharpe Ratio</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
         <v>0.281148392927856</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>0.214257967165815</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>-23.79185776786759</v>
       </c>
-      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -681,16 +726,21 @@
           <t>2011-01-01</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Min volatility (Markowitz)</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
         <v>-0.07945212136486937</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>-0.08284656781634053</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>4.272316954109741</v>
       </c>
-      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -706,16 +756,21 @@
           <t>2011-01-01</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Sharpe Ratio</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
         <v>-0.0456077190950445</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>-0.05749420356159388</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>26.06244009216613</v>
       </c>
-      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -731,16 +786,21 @@
           <t>2012-01-01</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Min volatility (Markowitz)</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
         <v>0.2149647504499653</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>0.2400181537129705</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>11.65465650092087</v>
       </c>
-      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -756,16 +816,21 @@
           <t>2012-01-01</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Sharpe Ratio</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
         <v>0.2494706860022564</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>0.3355077742319896</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>34.48785490931589</v>
       </c>
-      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -781,16 +846,21 @@
           <t>2013-01-01</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Min volatility (Markowitz)</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
         <v>0.2755726822910067</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>0.2150063970598403</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>-21.97833425564584</v>
       </c>
-      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -806,16 +876,21 @@
           <t>2013-01-01</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Sharpe Ratio</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
         <v>0.2820694477784019</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>0.2981098479233425</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>5.68668470522981</v>
       </c>
-      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -831,16 +906,21 @@
           <t>2014-01-01</t>
         </is>
       </c>
-      <c r="D16" t="n">
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Min volatility (Markowitz)</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
         <v>0.02973514714769785</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>0.06138097108671696</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>106.4256510379139</v>
       </c>
-      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -856,16 +936,21 @@
           <t>2014-01-01</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Sharpe Ratio</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
         <v>0.06794657137276688</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>0.06970152038944509</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>2.582836751320749</v>
       </c>
-      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -881,16 +966,21 @@
           <t>2015-01-01</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Min volatility (Markowitz)</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
         <v>0.1482403397952498</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>0.1940745277468003</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>30.91883627281001</v>
       </c>
-      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -906,16 +996,21 @@
           <t>2015-01-01</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Sharpe Ratio</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
         <v>0.1918503650708647</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>0.2075539619557382</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>8.185335940889651</v>
       </c>
-      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -931,16 +1026,21 @@
           <t>2016-01-01</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Min volatility (Markowitz)</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
         <v>0.1853763933461065</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>0.1457792223303653</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>-21.36041720361417</v>
       </c>
-      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -956,16 +1056,21 @@
           <t>2016-01-01</t>
         </is>
       </c>
-      <c r="D21" t="n">
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Sharpe Ratio</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
         <v>0.1853763933461065</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>0.157993832435027</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>-14.77133113705313</v>
       </c>
-      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -981,16 +1086,21 @@
           <t>2017-01-01</t>
         </is>
       </c>
-      <c r="D22" t="n">
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Min volatility (Markowitz)</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
         <v>0.09239168944298566</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>0.0984821062518698</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>6.591953070240695</v>
       </c>
-      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1006,16 +1116,21 @@
           <t>2017-01-01</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Sharpe Ratio</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
         <v>0.07684666475740871</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>0.1548357035063571</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>101.4865628783577</v>
       </c>
-      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1031,16 +1146,21 @@
           <t>2018-01-01</t>
         </is>
       </c>
-      <c r="D24" t="n">
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Min volatility (Markowitz)</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
         <v>-0.1666783906828535</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>-0.1410279615486639</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>-15.38917494289697</v>
       </c>
-      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1056,16 +1176,21 @@
           <t>2018-01-01</t>
         </is>
       </c>
-      <c r="D25" t="n">
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Sharpe Ratio</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
         <v>-0.1828382551107674</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>-0.1553214395131264</v>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>-15.04981306071353</v>
       </c>
-      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1081,16 +1206,21 @@
           <t>2019-01-01</t>
         </is>
       </c>
-      <c r="D26" t="n">
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Min volatility (Markowitz)</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
         <v>0.1744249743628245</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>0.1770669865086083</v>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>1.514698313951364</v>
       </c>
-      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1106,16 +1236,21 @@
           <t>2019-01-01</t>
         </is>
       </c>
-      <c r="D27" t="n">
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Sharpe Ratio</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
         <v>0.2409819098213731</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>0.2463952835761715</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>2.246381796380912</v>
       </c>
-      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1131,16 +1266,21 @@
           <t>2020-01-01</t>
         </is>
       </c>
-      <c r="D28" t="n">
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Min volatility (Markowitz)</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
         <v>0.01778692902880785</v>
       </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
         <v>0.01260987046669278</v>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>-29.10597188379322</v>
       </c>
-      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1156,16 +1296,21 @@
           <t>2020-01-01</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Sharpe Ratio</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
         <v>0.008625902340794991</v>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>0.03429541788627044</v>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>297.586438279913</v>
       </c>
-      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>